<commit_message>
Add logging for user authentication and HTTP requests; update user history with new session IDs
</commit_message>
<xml_diff>
--- a/user_data/admin_compliance/admin_compliance_retrieve.xlsx
+++ b/user_data/admin_compliance/admin_compliance_retrieve.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>time</t>
   </si>
@@ -55,6 +55,9 @@
     <t>2025-09-22 15:12:35.191698</t>
   </si>
   <si>
+    <t>2025-09-23 14:18:39.821885</t>
+  </si>
+  <si>
     <t>3b47e32c-002e-402a-a10d-81aed46c79c7</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t>e060705d-d5b0-4a85-908f-068e5c36d979</t>
   </si>
   <si>
+    <t>cd5a3b04-e765-4375-92fd-34ba54b29a07</t>
+  </si>
+  <si>
     <t>Mäuschen mach mal "piep"!</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
   </si>
   <si>
     <t>hallo</t>
+  </si>
+  <si>
+    <t>heya, how you doing?</t>
   </si>
   <si>
     <t xml:space="preserve">{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.016393441706895828}
@@ -142,6 +151,29 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">{'Doc_id': '460989726168196147', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '13 Protection from malicious software AND 13 Protection from malicious software &gt; 13.1 Measures against malicious software (proactive) AND 13 Protection from malicious software &gt; 13.2 Measures in case of suspected malware attack (reactive)', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[20, 21, 22, 23]]}", 'score': 0.03177805617451668}
+{'Doc_id': '460989726168196138', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '3 Acceptable use of company assets AND 3 Acceptable use of company assets &gt; 3.1 Physical access control AND 3 Acceptable use of company assets &gt; 3.1 Physical access control &gt; 3.1.1 Use of recording devices AND 3 Acceptable use of company assets &gt; 3.2 Logical access control AND 3 Acceptable use of company assets &gt; 3.2 Logical access control &gt; 3.2.1 Passwords AND 3 Acceptable use of company assets &gt; 3.3 Data access control AND 3 Acceptable use of company assets &gt; 3.3 Data access control &gt; 3.3.1 Internal and confidential information AND 3 Acceptable use of company assets &gt; 3.3 Data access control &gt; 3.3.2 Third-party business data AND 3 Acceptable use of company assets &gt; 3.4 Clean desk - clear screen AND 3 Acceptable use of company assets &gt; 3.4 Clean desk - clear screen &gt; 3.4.1 Clean desk AND 3 Acceptable use of company assets &gt; 3.4 Clean desk - clear screen &gt; 3.4.2 Clear screen AND 3 Acceptable use of company assets &gt; 3.5 Measures in case of suspected unauthorized use', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[6, 7, 8, 9]]}", 'score': 0.029286926612257957}
+{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.016393441706895828}
+{'Doc_id': '460989726168196165', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '3 Passwörter AND 3 Passwörter &gt; 3.1 Vertraulichkeit und Nutzung AND 3 Passwörter &gt; 3.2 Eigenschaften von Passwörtern', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[4, 5, 6]]}", 'score': 0.016129031777381897}
+{'Doc_id': '460989726168196169', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '6 Security-Token AND 6 Security-Token &gt; 6.1 Hardware-Token AND 6 Security-Token &gt; 6.2 Software-Token', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[9, 10, 11]]}", 'score': 0.01587301678955555}
+{'Doc_id': '460989726168196167', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '4 Personal Identification Numbers (PINs)', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[8]]}", 'score': 0.015625}
+{'Doc_id': '460989726168196196', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': 'Nicht erlaubt sind unter anderem AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.2 Internet AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.3 Internet-basierte Anwendungen und Cloud-Dienste AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.4 Kommunikations- und Steuerungssoftware AND · Passwort AND · Kontakte AND · Datenaustausch', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[18, 19, 20, 21]]}", 'score': 0.01515151560306549}
+{'Doc_id': '460989726168196155', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Leitlinie.pdf', 'Section': '3 Geltungsbereich', 'binary_hash': 'c107fb7abf32532523aee902fe8ea8036226974eb815e4597d5bde72c5b384eb', 'page_no': [[5]]}", 'score': 0.014925372786819935}
+{'Doc_id': '460989726168196170', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '7 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[11]]}", 'score': 0.014705882407724857}
+{'Doc_id': '460989726168196146', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '11 Email, internet, communication software and AI assistance systems AND 11 Email, internet, communication software and AI assistance systems &gt; 11.1 Email AND 11 Email, internet, communication software and AI assistance systems &gt; 11.2 Internet AND 11 Email, internet, communication software and AI assistance systems &gt; 11.3 Internet-based applications and Cloud services AND 11 Email, internet, communication software and AI assistance systems &gt; 11.4 Communication and control software AND 11 Email, internet, communication software and AI assistance systems &gt; 11.5 Use of AI assistance systems', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[17, 18, 19, 20]]}", 'score': 0.014492753893136978}
+{'Doc_id': '460989726168196161', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Leitlinie.pdf', 'Section': '8 Verpflichtung und Inkrafttreten', 'binary_hash': 'c107fb7abf32532523aee902fe8ea8036226974eb815e4597d5bde72c5b384eb', 'page_no': [[9, 10]]}", 'score': 0.014285714365541935}
+{'Doc_id': '460989726168196139', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '4 Data protection', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[9]]}", 'score': 0.014084506779909134}
+{'Doc_id': '460989726168196174', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Policy.pdf', 'Section': 'KISTERS Policy on Information Security, Data Protection AND and Business Continuity AND Table of contents AND 1 Introduction AND 2 Motivation and objectives AND 2 Motivation and objectives &gt; 2.1 Information security AND 2 Motivation and objectives &gt; 2.2 Data protection and privacy AND 2 Motivation and objectives &gt; 2.3 Business continuity AND 3 Scope', 'binary_hash': '80daf8c9a333576895bb99ef01545c6410c66e3fdb601ed7cc43ce3fef5de380', 'page_no': [[1, 2, 3, 4, 5]]}", 'score': 0.013888888992369175}
+{'Doc_id': '460989726168196186', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '3 Zulässige Nutzung von Unternehmenswerten &gt; 3.3 Zugriffskontrolle &gt; 3.3.2 Geschäftsdaten Dritter AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.4 Aufgeräumter Arbeitsplatz - leerer Bildschirm AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.4 Aufgeräumter Arbeitsplatz - leerer Bildschirm &gt; 3.4.1 Aufgeräumter Arbeitsplatz AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.4 Aufgeräumter Arbeitsplatz - leerer Bildschirm &gt; 3.4.2 Leerer Bildschirm AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.5 Maßnahmen beim Verdacht auf unberechtigte Nutzung', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[8, 9, 10]]}", 'score': 0.013698630034923553}
+{'Doc_id': '460989726168196193', 'Metadata': '{\'Date\': \'22-09-2025\', \'Document_Name\': \'KISTERS_IS_Richtlinie.pdf\', \'Section\': "9 Private Geräte und Medien - \'Restricted BYOD\'-Richtlinie AND 9 Private Geräte und Medien - \'Restricted BYOD\'-Richtlinie &gt; 9.1 Betriebliche Cloud-Dienste auf privaten Geräten", \'binary_hash\': \'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60\', \'page_no\': [[15, 16]]}', 'score': 0.013513513840734959}
+{'Doc_id': '460989726168196187', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '4 Datenschutz', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[10]]}", 'score': 0.013333333656191826}
+{'Doc_id': '460989726168196199', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '13 Schutz vor Schadsoftware &gt; 13.2 Maßnahmen bei Verdacht auf Befall durch Schadsoftware (reaktiv)', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.012987012974917889}
+{'Doc_id': '460989726168196185', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '3 Zulässige Nutzung von Unternehmenswerten AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.1 Zutrittskontrolle AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.1 Zutrittskontrolle &gt; 3.1.1 Nutzung von Aufzeichnungsgeräten AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.2 Zugangskontrolle AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.2 Zugangskontrolle &gt; 3.2.1 Passwörter AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.3 Zugriffskontrolle AND 3 Zulässige Nutzung von Unternehmenswerten &gt; 3.3 Zugriffskontrolle &gt; 3.3.1 Interne und Vertrauliche Information', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[6, 7, 8]]}", 'score': 0.012820512987673283}
+{'Doc_id': '460989726168196142', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '7 Procurement and Disposal of Data Storage Devices', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[11]]}", 'score': 0.012658228166401386}
+{'Doc_id': '460989726168196194', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '10 Netzwerkzugänge AND 10 Netzwerkzugänge &gt; 10.1 Zugang ins KISTERS Datennetz AND 10 Netzwerkzugänge &gt; 10.2 Zugang zum Internet AND 10 Netzwerkzugänge &gt; 10.3 Zugang zum Internet für Externe AND 10 Netzwerkzugänge &gt; 10.4 Zugänge zu externen Systemen / Fernwartungszugänge AND 10 Netzwerkzugänge &gt; 10.4 Zugänge zu externen Systemen / Fernwartungszugänge &gt; 10.4.1 Verbot der privaten Nutzung', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[16, 17, 18]]}", 'score': 0.012500000186264515}
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">{'Doc_id': '460989726168196198', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '13 Schutz vor Schadsoftware &gt; 13.1 Maßnahmen gegen Schadsoftware (proaktiv)', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[22, 23, 24, 25]]}", 'score': 0.0008745276559807254}
 {'Doc_id': '460989726168196196', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': 'Nicht erlaubt sind unter anderem AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.2 Internet AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.3 Internet-basierte Anwendungen und Cloud-Dienste AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.4 Kommunikations- und Steuerungssoftware AND · Passwort AND · Kontakte AND · Datenaustausch', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[18, 19, 20, 21]]}", 'score': 0.0006631049173202234}
 {'Doc_id': '460989726168196165', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '3 Passwörter AND 3 Passwörter &gt; 3.1 Vertraulichkeit und Nutzung AND 3 Passwörter &gt; 3.2 Eigenschaften von Passwörtern', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[4, 5, 6]]}", 'score': 0.0003379259420030768}
@@ -160,6 +192,12 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">{'Doc_id': '460989726168196199', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '13 Schutz vor Schadsoftware &gt; 13.2 Maßnahmen bei Verdacht auf Befall durch Schadsoftware (reaktiv)', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.00044056299756346925}
+{'Doc_id': '460989726168196146', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Guideline.pdf', 'Section': '11 Email, internet, communication software and AI assistance systems AND 11 Email, internet, communication software and AI assistance systems &gt; 11.1 Email AND 11 Email, internet, communication software and AI assistance systems &gt; 11.2 Internet AND 11 Email, internet, communication software and AI assistance systems &gt; 11.3 Internet-based applications and Cloud services AND 11 Email, internet, communication software and AI assistance systems &gt; 11.4 Communication and control software AND 11 Email, internet, communication software and AI assistance systems &gt; 11.5 Use of AI assistance systems', 'binary_hash': '1c0b642d21e992716a18d78dfbe53bc45781b8e4aa49625eec1064bce90ba0ca', 'page_no': [[17, 18, 19, 20]]}", 'score': 0.00042055616040459064}
+{'Doc_id': '460989726168196169', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '6 Security-Token AND 6 Security-Token &gt; 6.1 Hardware-Token AND 6 Security-Token &gt; 6.2 Software-Token', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[9, 10, 11]]}", 'score': 0.0003216020694962797}
+</t>
+  </si>
+  <si>
     <t>compliance_center</t>
   </si>
   <si>
@@ -176,6 +214,17 @@
   <si>
     <t xml:space="preserve">Hallo! Wie kann ich Ihnen heute behilflich sein? Ich bin Kisters AI-Assistent und stehe Ihnen für Fragen zu den Richtlinien und Informationen von Kister zur Verfügung. [INFO]
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heya! I'm doing well, thanks for asking! 😊 As a large language model, I don't experience emotions like humans do, but I'm functioning optimally and ready to help.
+Is there anything I can assist you with? [Source 1]
+</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -533,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -576,22 +625,22 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -599,22 +648,22 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -625,22 +674,54 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>28</v>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Batch Ingestion & Q
</commit_message>
<xml_diff>
--- a/user_data/admin_compliance/admin_compliance_retrieve.xlsx
+++ b/user_data/admin_compliance/admin_compliance_retrieve.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>time</t>
   </si>
@@ -61,6 +61,18 @@
     <t>2025-09-23 15:12:09.545096</t>
   </si>
   <si>
+    <t>2025-09-24 10:03:59.360276</t>
+  </si>
+  <si>
+    <t>2025-09-24 11:48:55.141417</t>
+  </si>
+  <si>
+    <t>2025-09-24 12:14:09.037715</t>
+  </si>
+  <si>
+    <t>2025-09-24 12:17:56.376608</t>
+  </si>
+  <si>
     <t>3b47e32c-002e-402a-a10d-81aed46c79c7</t>
   </si>
   <si>
@@ -76,6 +88,15 @@
     <t>aff7a446-a689-4d20-b0aa-0326a03fd033</t>
   </si>
   <si>
+    <t>c714b3d0-4a34-4a10-baf8-c4f540190c22</t>
+  </si>
+  <si>
+    <t>6978e8de-3644-48a6-8076-de07f9c86ed6</t>
+  </si>
+  <si>
+    <t>750f5463-a9b9-46a7-b2bd-3c618e334165</t>
+  </si>
+  <si>
     <t>Mäuschen mach mal "piep"!</t>
   </si>
   <si>
@@ -89,6 +110,18 @@
   </si>
   <si>
     <t>Welche Kriterien der ISO27002 werden von der Richtlinie zu Passwörtern abgedeckt?</t>
+  </si>
+  <si>
+    <t>Werden Controls aus der ISO 27019 in den bereitgestellten Richtlinien abgedeckt?</t>
+  </si>
+  <si>
+    <t>Was kannst du mir zur Organisation sagen?</t>
+  </si>
+  <si>
+    <t>Welche kryptographischen Standards sollten befolgt werden?</t>
+  </si>
+  <si>
+    <t>Wie sollten Dokumente der Sicherheitsstufe I3 vernichtet werden?</t>
   </si>
   <si>
     <t xml:space="preserve">{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.016393441706895828}
@@ -206,6 +239,98 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">{'Doc_id': '461014409579601599', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461032537848548007', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27017-2015.pdf', 'Section': '18 Compliance &gt; 18.2 Information security reviews AND 18 Compliance &gt; 18.2 Information security reviews &gt; 18.2.1 Independent review of information security', 'binary_hash': 'baa45e80a596e7eb929fd3450dcf1ea6f96ec07f6cca12aa0efe552c2fe0bf5a', 'page_no': [[35]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461014409579601543', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461032537848548023', 'Metadata': "{'Date': '19-08-2025', 'Document_Name': 'isoiec27018ed3.0en.pdf', 'Section': '5 Organizational controls &gt; 5.15 Access control', 'binary_hash': 'fd502230ea35a494108fa5a0852efba8aab5a74dbfabee2d128e530c21012e95', 'page_no': [[20, 21]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461014409579601572', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.6 Regelbetrieb (OPS) AND \\x84 OPS-01 Kapazitätsmanagement - Planung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OPS-02 Kapazitätsmanagement - Überwachung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 OPS-03 Kapazitätsmanagement - Steuerung von Ressourcen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 OPS-04 Schutz vor Schadprogrammen Konzept AND Basiskriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[63, 64, 65]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461032537848547999', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27017-2015.pdf', 'Section': '7 Human resource security &gt; 7.2 During employment &gt; 7.2.2 Information security awareness, education and training', 'binary_hash': 'baa45e80a596e7eb929fd3450dcf1ea6f96ec07f6cca12aa0efe552c2fe0bf5a', 'page_no': [[18]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461014409579601516', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.6 Regelbetrieb (OPS) AND \\x84 OPS-01 Kapazitätsmanagement - Planung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OPS-02 Kapazitätsmanagement - Überwachung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 OPS-03 Kapazitätsmanagement - Steuerung von Ressourcen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 OPS-04 Schutz vor Schadprogrammen Konzept AND Basiskriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[63, 64, 65]]}", 'score': 0.015625}
+{'Doc_id': '461032537848547997', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27017-2015.pdf', 'Section': '5 Information security policies AND 5 Information security policies &gt; 5.1 Management direction for information security AND 5 Information security policies &gt; 5.1 Management direction for information security &gt; 5.1.1 Policies for information security', 'binary_hash': 'baa45e80a596e7eb929fd3450dcf1ea6f96ec07f6cca12aa0efe552c2fe0bf5a', 'page_no': [[16]]}", 'score': 0.015625}
+{'Doc_id': '461014409579601416', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[13]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461014409579601564', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.2 Sicherheitsrichtlinien und Arbeitsanweisungen (SP) AND \\x84 SP-01 Dokumentation, Kommunikation und Bereitstellung von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 SP-02 Überprüfung und Freigabe von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[43, 44, 45, 46]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461014409579601419', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 &gt; 3.1.3 3 &gt; 3.1.3 4 &gt; 3.1.3 5 &gt; 3.1.3 6 &gt; 3.1.3 7', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[16]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601508', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.2 Sicherheitsrichtlinien und Arbeitsanweisungen (SP) AND \\x84 SP-01 Dokumentation, Kommunikation und Bereitstellung von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 SP-02 Überprüfung und Freigabe von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[43, 44, 45, 46]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601465', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '8 Technological controls &gt; 8.33 Test information', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[139]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601566', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 HR-04 Maßregelungsprozess AND Basiskriterium AND Ergänzende Informationen AND \\x84 HR-05 Verantwortlichkeiten bei Beendigung oder Änderung der Beschäftigung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: ja AND \\x84 HR-06 Vertraulichkeitsvereinbarungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: ja AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.4 Asset Management (AM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[48, 49, 50, 51]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601458', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '8 Technological controls &gt; 8.19 Installation of software on operational systems', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[120]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461014409579601510', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 HR-04 Maßregelungsprozess AND Basiskriterium AND Ergänzende Informationen AND \\x84 HR-05 Verantwortlichkeiten bei Beendigung oder Änderung der Beschäftigung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: ja AND \\x84 HR-06 Vertraulichkeitsvereinbarungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: ja AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.4 Asset Management (AM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[48, 49, 50, 51]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461014409579601584', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Korrespondierende Kriterien für Kunden AND Möglichkeit: nein AND \\x84 COS-07 Dokumentation des Netzes AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 COS-08 Richtlinien zur Datenübertragung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Korrespondierende Kriterien für Kunden AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.10 Portabilität und Interoperabilität (PI) AND \\x84 PI-01 Dokumentation und Sicherheit der Eingangs- und Ausgangs-Schnittstellen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: teilweise AND \\x84 PI-02 Vertragliche Vereinbarungen zur Bereitstellung von Daten AND Basiskriterium AND Zusatzkriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[93, 94, 95]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461032537848547989', 'Metadata': "{'Date': '02-10-2024', 'Document_Name': 'INV 17096 ISO 27019 2024.pdf', 'Section': 'ISO/IEC 27019:2024(en)', 'binary_hash': '37e5cc120d33926bd388cadc4d9b0efe2904be72a16f027719d2a54fef7f5d86', 'page_no': [[47, 48]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461014409579601448', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '8 Technological controls &gt; 8.3 Information access restriction', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[94]]}", 'score': 0.014285714365541935}
+{'Doc_id': '461014409579601528', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Korrespondierende Kriterien für Kunden AND Möglichkeit: nein AND \\x84 COS-07 Dokumentation des Netzes AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 COS-08 Richtlinien zur Datenübertragung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Korrespondierende Kriterien für Kunden AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.10 Portabilität und Interoperabilität (PI) AND \\x84 PI-01 Dokumentation und Sicherheit der Eingangs- und Ausgangs-Schnittstellen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: teilweise AND \\x84 PI-02 Vertragliche Vereinbarungen zur Bereitstellung von Daten AND Basiskriterium AND Zusatzkriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[93, 94, 95]]}", 'score': 0.014285714365541935}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461014409579601411', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'Foreword AND Introduction AND 0.1 Background and context AND 0.2 Information security requirements AND 0.3 Controls AND 0.4 Determining controls', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[6, 7, 8]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461032537848547991', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27017-2015.pdf', 'Section': 'INTERNATIONAL STANDARD AND COPYRIGHT PROTECTED DOCUMENT AND 2015 © ISO/IEC AND Foreword AND ITU-T AND ITU-T X-SERIES RECOMMENDATIONS AND DATA NETWORKS, OPEN SYSTEM COMMUNICATIONS AND SECURITY AND INTERNATIONAL STANDARD ISO/IEC 27017 RECOMMENDATION ITU-T X.1631 AND Information technology - Security techniques - Code of practice for information security controls based on ISO/IEC 27002 for cloud services', 'binary_hash': 'baa45e80a596e7eb929fd3450dcf1ea6f96ec07f6cca12aa0efe552c2fe0bf5a', 'page_no': [[1, 2, 3, 4, 5, 6, 7]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461014409579601545', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Vorwort des Präsidenten', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[3]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461032537848547989', 'Metadata': "{'Date': '02-10-2024', 'Document_Name': 'INV 17096 ISO 27019 2024.pdf', 'Section': 'ISO/IEC 27019:2024(en)', 'binary_hash': '37e5cc120d33926bd388cadc4d9b0efe2904be72a16f027719d2a54fef7f5d86', 'page_no': [[47, 48]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461014409579601489', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Vorwort des Präsidenten', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[3]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461014409579601543', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.01587301678955555}
+{'Doc_id': '460989726168196164', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': 'KISTERS Passwortrichtlinie Identitätsmanagement und Authentisierung AND Inhaltsverzeichnis AND 1 Einleitung AND 1 Einleitung &gt; 1.1 Motivation und Ziele AND 1 Einleitung &gt; 1.2 Anwendungsbereich AND 1 Einleitung &gt; 1.3 Rollen, Verantwortlichkeiten und Abhängigkeiten AND 1 Einleitung &gt; 1.4 Anwendbare rechtliche und regulatorische Anforderungen AND 2 Generelle Vorgaben AND Grundsätzlich gilt:', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[1, 2, 3, 4]]}", 'score': 0.015625}
+{'Doc_id': '461014409579601599', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.015625}
+{'Doc_id': '461014409579601482', 'Metadata': "{'Date': '29-09-2022', 'Document_Name': 'ISO_IEC 27001_2022_ Information security, cybersecurity and -- ISO -- 2022-10, 3, 2022 -- ISO -- c40db4f08bbcd7ac67a02553fcb47a70 -- Annas Archive.pdf', 'Section': '7 Support AND 7 Support &gt; 7.1 Resources AND 7 Support &gt; 7.2 Competence AND 7 Support &gt; 7.3 Awareness AND 7 Support &gt; 7.4 Communication AND 7 Support &gt; 7.5 Documented information AND 7 Support &gt; 7.5 Documented information &gt; 7.5.1 General AND 7 Support &gt; 7.5 Documented information &gt; 7.5.2 Creating and updating AND 7 Support &gt; 7.5 Documented information &gt; 7.5.3 Control of documented information', 'binary_hash': 'e739019c5c1ac8c6f1a761d2ac2cf2107847833822ffc7808dd885d90ec9529b', 'page_no': [[12, 13]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461014409579601551', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2.2 Inhaltliche Gliederung der C5-Kriterien', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[18, 19]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461014409579601418', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'privacy impact assessment AND process AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 &gt; 3.1.2 1 &gt; 3.1.2 2 &gt; 3.1.2 4 &gt; 3.1.2 8 AND record AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 &gt; 3.1.2 1 &gt; 3.1.2 2 &gt; 3.1.2 4 &gt; 3.1.2 8 &gt; 3.1.2 9 AND recovery point objective AND RPO AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 AND recovery time objective AND RTO AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 AND reliability AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 AND rule AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 &gt; 3.1.3 3 AND sensitive information AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 &gt; 3.1.3 3 &gt; 3.1.3 4 AND threat AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 &gt; 3.1.3 3 &gt; 3.1.3 4 &gt; 3.1.3 5 AND topic-specific\\tpolicy AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.3 0 &gt; 3.1.3 1 &gt; 3.1.3 2 &gt; 3.1.3 3 &gt; 3.1.3 4 &gt; 3.1.3 5 &gt; 3.1.3 6 AND user AND ISO/IEC 27002:2022(E)', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[14, 15, 16]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601495', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2.2 Inhaltliche Gliederung der C5-Kriterien', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[18, 19]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601415', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'Information security, cybersecurity and privacy protection - Information security controls AND 1 Scope AND 2 Normative references AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 AND access control AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 AND asset AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 AND attack AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 AND authentication AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 AND authenticity AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 AND chain of custody AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 AND confidential\\tinformation AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 AND control AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 AND disruption AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 AND endpoint device AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 AND entity AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 AND information processing facility AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 AND information security breach', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[11, 12, 13]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601562', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND \\x84 BC-06 Angaben zu Zertifizierungen oder Bescheinigungen AND Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.1 Organisation der Informationssicherheit (OIS) AND Ergänzende Informationen AND \\x84 OIS-02 Leitlinie zur Informationssicherheit AND Basiskriterium AND \\x84 OIS-01 Informations  sicherheits  managementsystem (ISMS) AND Basiskriterium AND Zusatzkriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OIS-03 Schnittstellen und Abhängigkeiten AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[36, 37, 38, 39, 40]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601417', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'information security event AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4 &gt; 3.1.1 5 AND information security incident AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4 &gt; 3.1.1 5 &gt; 3.1.1 6 AND information security incident management AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4 &gt; 3.1.1 5 &gt; 3.1.1 6 &gt; 3.1.1 7 AND information system AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4 &gt; 3.1.1 5 &gt; 3.1.1 6 &gt; 3.1.1 7 &gt; 3.1.1 8 AND interested party AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.1 0 &gt; 3.1.1 1 &gt; 3.1.1 2 &gt; 3.1.1 3 &gt; 3.1.1 4 &gt; 3.1.1 5 &gt; 3.1.1 6 &gt; 3.1.1 7 &gt; 3.1.1 8 &gt; 3.1.1 9 AND non-repudiation AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 AND personnel AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 &gt; 3.1.2 1 AND personally\\tidentifiable\\tinformation AND PII AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 &gt; 3.1.2 1 &gt; 3.1.2 2 AND PII principal AND PII processor AND 3 Terms,\\tdefinitions\\tand\\tabbreviated\\tterms &gt; 3.1 Terms\\tand\\tdefinitions &gt; 3.1 .1 &gt; 3.1 .2 &gt; 3.1 .3 &gt; 3.1 .4 &gt; 3.1 .5 &gt; 3.1 .6 &gt; 3.1 .7 &gt; 3.1 .8 &gt; 3.1 .9 &gt; 3.1.2 0 &gt; 3.1.2 1 &gt; 3.1.2 2 &gt; 3.1.2 4', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[13, 14]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461014409579601506', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND \\x84 BC-06 Angaben zu Zertifizierungen oder Bescheinigungen AND Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.1 Organisation der Informationssicherheit (OIS) AND Ergänzende Informationen AND \\x84 OIS-02 Leitlinie zur Informationssicherheit AND Basiskriterium AND \\x84 OIS-01 Informations  sicherheits  managementsystem (ISMS) AND Basiskriterium AND Zusatzkriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OIS-03 Schnittstellen und Abhängigkeiten AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[36, 37, 38, 39, 40]]}", 'score': 0.014705882407724857}
+{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461014409579601548', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '1 Einleitung AND 1 Einleitung &gt; 1 Einleitung AND 1 Einleitung &gt; 1 Einleitung &gt; 1.1 Vorbemerkungen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[12, 13, 14]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461014409579601492', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '1 Einleitung AND 1 Einleitung &gt; 1 Einleitung AND 1 Einleitung &gt; 1 Einleitung &gt; 1.1 Vorbemerkungen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[12, 13, 14]]}", 'score': 0.014285714365541935}
+{'Doc_id': '461014409579601579', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND \\x84 IDM-03 Sperrung und Entzug von Zugangsberechtigungen bei Inaktivität oder mehrfach fehlgeschlagenen Anmeldungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Ergänzende Informationen AND \\x84 IDM-04 Entzug oder Anpassung von Zugriffsberechtigungen bei Veränderungen des Aufgabengebiets AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: ja AND \\x84 IDM-05 Regelmäßige Überprüfung der Zugriffsberechtigungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Korrespondierende Kriterien für Kunden AND Möglichkeit: ja AND \\x84 IDM-06 Privilegierte Zugriffsberechtigungen AND Basiskriterium AND Zusatzkriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[81, 82, 83]]}", 'score': 0.014285714365541935}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461014409579601585', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 PI-03 Sichere Datenlöschung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.11 Beschaffung, Entwicklung und Änderung von Informationssystemen (DEV) AND \\x84 DEV-01 Richtlinien zur Entwicklung/ Beschaffung von Informationssystemen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 DEV-02 Auslagerung der Entwicklung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[96, 97, 98]]}", 'score': 0.029323630034923553}
+{'Doc_id': '461014409579601529', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 PI-03 Sichere Datenlöschung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.11 Beschaffung, Entwicklung und Änderung von Informationssystemen (DEV) AND \\x84 DEV-01 Richtlinien zur Entwicklung/ Beschaffung von Informationssystemen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 DEV-02 Auslagerung der Entwicklung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[96, 97, 98]]}", 'score': 0.0292735043913126}
+{'Doc_id': '461014409579601582', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 CRY-04 Sichere Schlüsselverwaltung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.9 Kommunikationssicherheit (COS) AND \\x84 COS-01 Technische Schutzmaßnahmen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Hinweise zur kontinuierlichen Prüfung AND \\x84 COS-02 Sicherheitsanforderungen an Verbindungen im Netz des Cloud-Anbieters AND Basiskriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[88, 89, 90]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461034822404409041', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '7 Referenzen', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[15, 16, 17]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461014409579601411', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'Foreword AND Introduction AND 0.1 Background and context AND 0.2 Information security requirements AND 0.3 Controls AND 0.4 Determining controls', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[6, 7, 8]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461014409579601526', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 CRY-04 Sichere Schlüsselverwaltung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.9 Kommunikationssicherheit (COS) AND \\x84 COS-01 Technische Schutzmaßnahmen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Hinweise zur kontinuierlichen Prüfung AND \\x84 COS-02 Sicherheitsanforderungen an Verbindungen im Netz des Cloud-Anbieters AND Basiskriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[88, 89, 90]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461014409579601534', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.13 Umgang mit Sicherheitsvorfällen (SIM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[108]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461034822404409038', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '5 Kryptographische Verfahren &gt; 5.2 Auswahl starker kryptographischer Algorithmen &gt; 5.2.2 Bekannte schwache Algorithmen AND 5 Kryptographische Verfahren &gt; 5.2 Auswahl starker kryptographischer Algorithmen &gt; 5.2.3 Kontinuierliche Neubewertung', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[13, 14]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461014409579601590', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.13 Umgang mit Sicherheitsvorfällen (SIM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[108]]}", 'score': 0.015625}
+{'Doc_id': '461032537848547989', 'Metadata': "{'Date': '02-10-2024', 'Document_Name': 'INV 17096 ISO 27019 2024.pdf', 'Section': 'ISO/IEC 27019:2024(en)', 'binary_hash': '37e5cc120d33926bd388cadc4d9b0efe2904be72a16f027719d2a54fef7f5d86', 'page_no': [[47, 48]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461034289014768777', 'Metadata': "{'Date': '05-08-2025', 'Document_Name': 'KISTERS_IS_LawsRegulations.pdf', 'Section': '5 Data Protection / Privacy &gt; 5.3 Telecommunications and Digital ServicesData Protection Act / Telekommunikation-Digitale-Dienste-Datenschutz-Gesetz (TDDDG) &gt; 5.3.2 Relevant Topics AND 5 Data Protection / Privacy &gt; 5.4 EU Geoblocking Regulation / EU Geoblocking Verordnung AND 5 Data Protection / Privacy &gt; 5.4 EU Geoblocking Regulation / EU Geoblocking Verordnung &gt; 5.4.1 Links AND 5 Data Protection / Privacy &gt; 5.4 EU Geoblocking Regulation / EU Geoblocking Verordnung &gt; 5.4.2 Relevant Topics', 'binary_hash': '585533c734593d00c08f1a4e33367aafba212325f74df2b4babeb0346aa8627a', 'page_no': [[19, 20, 21]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461034822404409031', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': 'KISTERS Kryptographie Richtlinie AND zu kryptographischen Maßnahmen AND Inhaltsverzeichnis AND 1.1 Anwendungsbereich AND 1.2 Rollen, Verantwortlichkeiten und Abhängigkeiten AND 1.3 Anwendbare rechtliche und regulatorische Anforderungen AND 2 Anwendung der Kryptographie', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[1, 2, 3, 4]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601543', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601573', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OPS-05 Schutz vor Schadprogrammen Umsetzung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND \\x84 OPS-06 Vorgaben zur Datensicherung und Wiederherstellung - Konzept AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Möglichkeit: teilweise AND \\x84 OPS-07 Datensicherung und Wiederherstellung - Überwachung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[65, 66, 67, 68]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601517', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OPS-05 Schutz vor Schadprogrammen Umsetzung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND \\x84 OPS-06 Vorgaben zur Datensicherung und Wiederherstellung - Konzept AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Korrespondierende Kriterien für Kunden AND Möglichkeit: teilweise AND \\x84 OPS-07 Datensicherung und Wiederherstellung - Überwachung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[65, 66, 67, 68]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461014409579601599', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461032537848548026', 'Metadata': "{'Date': '19-08-2025', 'Document_Name': 'isoiec27018ed3.0en.pdf', 'Section': 'ISO/IEC 27018:2025(en) AND 7 Physical controls &gt; 7.13 Equipment maintenance AND 7 Physical controls &gt; 7.14 Secure disposal or re-use of equipment AND 8 Technological controls AND 8 Technological controls &gt; 8.1 User endpoint devices AND 8 Technological controls &gt; 8.2 Privileged access rights AND 8 Technological controls &gt; 8.3 Information access restriction AND 8 Technological controls &gt; 8.4 Access to source code AND 8 Technological controls &gt; 8.5 Secure authentication AND 8 Technological controls &gt; 8.6 Capacity management AND 8 Technological controls &gt; 8.7 Protection against malware AND 8 Technological controls &gt; 8.8 Management of technical vulnerabilities AND ISO/IEC 27018:2025(en) AND 8 Technological controls &gt; 8.9 Configuration management AND 8 Technological controls &gt; 8.10 Information deletion AND 8 Technological controls &gt; 8.11 Data masking AND 8 Technological controls &gt; 8.12 Data leakage prevention AND 8 Technological controls &gt; 8.13 Information backup AND a) Public cloud PII protection implementation guidance AND ISO/IEC 27018:2025(en) AND 8 Technological controls &gt; 8.14 Redundancy of information processing facilities AND 8 Technological controls &gt; 8.15 Logging AND 8 Technological controls &gt; 8.16 Monitoring activities AND 8 Technological controls &gt; 8.17 Clock synchronization AND 8 Technological controls &gt; 8.18 Use of privileged utility programs AND 8 Technological controls &gt; 8.19 Installation of software on operational systems AND 8 Technological controls &gt; 8.20 Networks security AND 8 Technological controls &gt; 8.21 Security of network services', 'binary_hash': 'fd502230ea35a494108fa5a0852efba8aab5a74dbfabee2d128e530c21012e95', 'page_no': [[25, 26, 27, 28]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461034822404409033', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '2 Anwendung der Kryptographie &gt; 2.4 Softwareentwicklung AND 2 Anwendung der Kryptographie &gt; 2.5 Auswahl von Kryptographieprodukten AND 2 Anwendung der Kryptographie &gt; 2.6 Einschränkungen', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[6, 7]]}", 'score': 0.014492753893136978}
+{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.014285714365541935}
+{'Doc_id': '461014409579601589', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Hinweise zur kontinuierlichen Prüfung AND \\x84 SSO-04 Überwachung der Einhaltung der Anforderungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND \\x84 SSO-05 Ausstiegsstrategie für den Bezug von Leistungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[106, 107, 108]]}", 'score': 0.014285714365541935}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461014409579601529', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 PI-03 Sichere Datenlöschung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.11 Beschaffung, Entwicklung und Änderung von Informationssystemen (DEV) AND \\x84 DEV-01 Richtlinien zur Entwicklung/ Beschaffung von Informationssystemen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 DEV-02 Auslagerung der Entwicklung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[96, 97, 98]]}", 'score': 0.027222223579883575}
+{'Doc_id': '461014409579601585', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 PI-03 Sichere Datenlöschung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.11 Beschaffung, Entwicklung und Änderung von Informationssystemen (DEV) AND \\x84 DEV-01 Richtlinien zur Entwicklung/ Beschaffung von Informationssystemen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 DEV-02 Auslagerung der Entwicklung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[96, 97, 98]]}", 'score': 0.027212142944335938}
+{'Doc_id': '460989726168196131', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '6 Klassifikationskriterien &gt; 6.2 Datenvernichtung nach DIN 66399 / ISO 21964-1', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[26, 27]]}", 'score': 0.016393441706895828}
+{'Doc_id': '461014409579601534', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.13 Umgang mit Sicherheitsvorfällen (SIM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[108]]}", 'score': 0.016393441706895828}
+{'Doc_id': '460989726168196126', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '5 Zugriffskontrolle AND 5 Zugriffskontrolle &gt; 5.1 Klassifikation von Information AND 5 Zugriffskontrolle &gt; 5.2 Zugriffsberechtigungen AND 5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung AND 5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung &gt; 5.3.1 Öffentlich (I0)', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[19, 20, 21, 22]]}", 'score': 0.016129031777381897}
+{'Doc_id': '461014409579601590', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.13 Umgang mit Sicherheitsvorfällen (SIM)', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[108]]}", 'score': 0.016129031777381897}
+{'Doc_id': '460989726168196200', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '14 Meldungen von Sicherheitsereignissen und -vorfällen', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[25]]}", 'score': 0.01587301678955555}
+{'Doc_id': '461034822404409032', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '2 Anwendung der Kryptographie &gt; 2.1 Grundsätzliche Maßnahmen AND 2 Anwendung der Kryptographie &gt; 2.2 Algorithmen AND 2 Anwendung der Kryptographie &gt; 2.3 Schutz von Daten beim Transport und im Ruhezustand', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[4, 5, 6]]}", 'score': 0.01587301678955555}
+{'Doc_id': '460989726168196196', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': 'Nicht erlaubt sind unter anderem AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.2 Internet AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.3 Internet-basierte Anwendungen und Cloud-Dienste AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.4 Kommunikations- und Steuerungssoftware AND · Passwort AND · Kontakte AND · Datenaustausch', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[18, 19, 20, 21]]}", 'score': 0.015625}
+{'Doc_id': '461014409579601411', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': 'Foreword AND Introduction AND 0.1 Background and context AND 0.2 Information security requirements AND 0.3 Controls AND 0.4 Determining controls', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[6, 7, 8]]}", 'score': 0.015625}
+{'Doc_id': '460989726168196128', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung &gt; 5.3.4 Vertraulich (I3)', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[23, 24]]}", 'score': 0.015384615398943424}
+{'Doc_id': '461014409579601543', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.015384615398943424}
+{'Doc_id': '460989726168196115', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': 'KISTERS Klassifikation der Informationswerte - AND Zutritts-, Zugangs- und Zugriffskontrolle AND Inhaltsverzeichnis AND 1 Einleitung AND 1 Einleitung &gt; 1.1 Motivation und Ziele AND 1 Einleitung &gt; 1.2 Anwendungsbereich', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[1, 2, 3, 4]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601599', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Errata AND Herausgeber: AND Bezugsquelle: AND Stand: AND Angaben zur Druckerei: AND Texte und Redaktion: AND Bildnachweis: AND Artikelnummer:', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[130, 131]]}", 'score': 0.01515151560306549}
+{'Doc_id': '461014409579601597', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND \\x84 PSS-06 Session Management AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 PSS-07 Vertraulichkeit von AND Authentisierungsinformationen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND \\x84 PSS-08 Rollen- und Rechtekonzept AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 PSS-09 Autorisierungsmechanismen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[124, 125, 126, 127]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461032537848547989', 'Metadata': "{'Date': '02-10-2024', 'Document_Name': 'INV 17096 ISO 27019 2024.pdf', 'Section': 'ISO/IEC 27019:2024(en)', 'binary_hash': '37e5cc120d33926bd388cadc4d9b0efe2904be72a16f027719d2a54fef7f5d86', 'page_no': [[47, 48]]}", 'score': 0.014925372786819935}
+{'Doc_id': '461014409579601482', 'Metadata': "{'Date': '29-09-2022', 'Document_Name': 'ISO_IEC 27001_2022_ Information security, cybersecurity and -- ISO -- 2022-10, 3, 2022 -- ISO -- c40db4f08bbcd7ac67a02553fcb47a70 -- Annas Archive.pdf', 'Section': '7 Support AND 7 Support &gt; 7.1 Resources AND 7 Support &gt; 7.2 Competence AND 7 Support &gt; 7.3 Awareness AND 7 Support &gt; 7.4 Communication AND 7 Support &gt; 7.5 Documented information AND 7 Support &gt; 7.5 Documented information &gt; 7.5.1 General AND 7 Support &gt; 7.5 Documented information &gt; 7.5.2 Creating and updating AND 7 Support &gt; 7.5 Documented information &gt; 7.5.3 Control of documented information', 'binary_hash': 'e739019c5c1ac8c6f1a761d2ac2cf2107847833822ffc7808dd885d90ec9529b', 'page_no': [[12, 13]]}", 'score': 0.014705882407724857}
+{'Doc_id': '461014409579601541', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen AND \\x84 PSS-06 Session Management AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 PSS-07 Vertraulichkeit von AND Authentisierungsinformationen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Zum Kriterium AND \\x84 PSS-08 Rollen- und Rechtekonzept AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND Möglichkeit: teilweise AND \\x84 PSS-09 Autorisierungsmechanismen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[124, 125, 126, 127]]}", 'score': 0.014705882407724857}
+{'Doc_id': '460989726168196198', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '13 Schutz vor Schadsoftware &gt; 13.1 Maßnahmen gegen Schadsoftware (proaktiv)', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[22, 23, 24, 25]]}", 'score': 0.014492753893136978}
+{'Doc_id': '461014409579601563', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Zum Kriterium AND Korrespondierende Kriterien für Kunden AND \\x84 OIS-04 Aufgabentrennung AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 OIS-05 Kontakt zu relevanten Behörden und Interessenverbänden AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Möglichkeit: ja AND \\x84 OIS-06 Richtlinie für den Umgang mit Risiken AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Korrespondierende Kriterien für Kunden AND Möglichkeit: teilweise AND \\x84 OIS-07 Anwendung des Verfahrens für den Umgang mit Risiken', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[40, 41, 42, 43]]}", 'score': 0.014492753893136978}
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">{'Doc_id': '460989726168196198', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': '13 Schutz vor Schadsoftware &gt; 13.1 Maßnahmen gegen Schadsoftware (proaktiv)', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[22, 23, 24, 25]]}", 'score': 0.0008745276559807254}
 {'Doc_id': '460989726168196196', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Richtlinie.pdf', 'Section': 'Nicht erlaubt sind unter anderem AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.2 Internet AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.3 Internet-basierte Anwendungen und Cloud-Dienste AND 11 E-Mail,  Internet, Kommunikationssoftware und KI-Assistenzsysteme &gt; 11.4 Kommunikations- und Steuerungssoftware AND · Passwort AND · Kontakte AND · Datenaustausch', 'binary_hash': 'bc1e0610f1a4ffd3bbe9faae98f27eab87bd95a5d6de1bbdd484f88c38c4fd60', 'page_no': [[18, 19, 20, 21]]}", 'score': 0.0006631049173202234}
 {'Doc_id': '460989726168196165', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': '3 Passwörter AND 3 Passwörter &gt; 3.1 Vertraulichkeit und Nutzung AND 3 Passwörter &gt; 3.2 Eigenschaften von Passwörtern', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[4, 5, 6]]}", 'score': 0.0003379259420030768}
@@ -233,6 +358,30 @@
     <t xml:space="preserve">{'Doc_id': '460989726168196164', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_PasswortRichtlinie.pdf', 'Section': 'KISTERS Passwortrichtlinie Identitätsmanagement und Authentisierung AND Inhaltsverzeichnis AND 1 Einleitung AND 1 Einleitung &gt; 1.1 Motivation und Ziele AND 1 Einleitung &gt; 1.2 Anwendungsbereich AND 1 Einleitung &gt; 1.3 Rollen, Verantwortlichkeiten und Abhängigkeiten AND 1 Einleitung &gt; 1.4 Anwendbare rechtliche und regulatorische Anforderungen AND 2 Generelle Vorgaben AND Grundsätzlich gilt:', 'binary_hash': 'fd6c1a1d68197f65661ca7c7d1ed2ed8e9cf3cbc738a53bbd9cd2057da3a2427', 'page_no': [[1, 2, 3, 4]]}", 'score': 0.25113144361542034}
 {'Doc_id': '461014409579601425', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '5 Organizational controls &gt; 5.12 Classification\\tof\\tinformation', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[32]]}", 'score': 0.012443839297313216}
 {'Doc_id': '461014409579601552', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2.3 Zugrundeliegende Standards und Publikationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[20, 21]]}", 'score': 0.011965652409114184}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461032537848547989', 'Metadata': "{'Date': '02-10-2024', 'Document_Name': 'INV 17096 ISO 27019 2024.pdf', 'Section': 'ISO/IEC 27019:2024(en)', 'binary_hash': '37e5cc120d33926bd388cadc4d9b0efe2904be72a16f027719d2a54fef7f5d86', 'page_no': [[47, 48]]}", 'score': 0.018730065246014817}
+{'Doc_id': '461014409579601458', 'Metadata': "{'Date': 'N/A', 'Document_Name': 'ISO IEC 27002 Information security, cybersecurity and -- Joint Technical Committee ISO_IEC JTC 1, Information -- International standard ISO_IEC -- a967f3067ce6b698454eb51ae20b6acb -- Annas Archive.pdf', 'Section': '8 Technological controls &gt; 8.19 Installation of software on operational systems', 'binary_hash': '120898d1de7720cf8c5180536a983edce0731b1c233af5932d2be1f9c8051987', 'page_no': [[120]]}", 'score': 0.01831900612196869}
+{'Doc_id': '461014409579601564', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.2 Sicherheitsrichtlinien und Arbeitsanweisungen (SP) AND \\x84 SP-01 Dokumentation, Kommunikation und Bereitstellung von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND \\x84 SP-02 Überprüfung und Freigabe von Richtlinien und Anweisungen AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[43, 44, 45, 46]]}", 'score': 0.016748181605773405}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461014409579601562', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND \\x84 BC-06 Angaben zu Zertifizierungen oder Bescheinigungen AND Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.1 Organisation der Informationssicherheit (OIS) AND Ergänzende Informationen AND \\x84 OIS-02 Leitlinie zur Informationssicherheit AND Basiskriterium AND \\x84 OIS-01 Informations  sicherheits  managementsystem (ISMS) AND Basiskriterium AND Zusatzkriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OIS-03 Schnittstellen und Abhängigkeiten AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[36, 37, 38, 39, 40]]}", 'score': 0.0010393486747203755}
+{'Doc_id': '461014409579601562', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': 'Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND \\x84 BC-06 Angaben zu Zertifizierungen oder Bescheinigungen AND Ergänzende Informationen - Hinweise zu den Rahmenbedingungen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen AND 5 Basiskriterien, Zusatzkriterien und ergänzende Informationen &gt; 5.1 Organisation der Informationssicherheit (OIS) AND Ergänzende Informationen AND \\x84 OIS-02 Leitlinie zur Informationssicherheit AND Basiskriterium AND \\x84 OIS-01 Informations  sicherheits  managementsystem (ISMS) AND Basiskriterium AND Zusatzkriterium AND Zusatzkriterium AND Ergänzende Informationen AND Hinweise zur kontinuierlichen Prüfung AND \\x84 OIS-03 Schnittstellen und Abhängigkeiten AND Basiskriterium AND Zusatzkriterium AND Ergänzende Informationen', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[36, 37, 38, 39, 40]]}", 'score': 0.0010393486747203755}
+{'Doc_id': '461014409579601551', 'Metadata': "{'Date': '11-12-2020', 'Document_Name': 'C5_2020.pdf', 'Section': '2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2 Aufbau und inhaltliche Gliederung der Kriterien &gt; 2.2 Inhaltliche Gliederung der C5-Kriterien', 'binary_hash': '93e4d583961bd2c70399cc7ca08dfc024131b93f120dcb3cd38c488c29a4eec3', 'page_no': [[18, 19]]}", 'score': 0.0007601554153838224}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '461034822404409033', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '2 Anwendung der Kryptographie &gt; 2.4 Softwareentwicklung AND 2 Anwendung der Kryptographie &gt; 2.5 Auswahl von Kryptographieprodukten AND 2 Anwendung der Kryptographie &gt; 2.6 Einschränkungen', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[6, 7]]}", 'score': 0.5206825943356754}
+{'Doc_id': '461034822404409031', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': 'KISTERS Kryptographie Richtlinie AND zu kryptographischen Maßnahmen AND Inhaltsverzeichnis AND 1.1 Anwendungsbereich AND 1.2 Rollen, Verantwortlichkeiten und Abhängigkeiten AND 1.3 Anwendbare rechtliche und regulatorische Anforderungen AND 2 Anwendung der Kryptographie', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[1, 2, 3, 4]]}", 'score': 0.16178945093564964}
+{'Doc_id': '461034822404409041', 'Metadata': "{'Date': '28-07-2025', 'Document_Name': 'KISTERS_IS_Kryptographie.pdf', 'Section': '7 Referenzen', 'binary_hash': '66f9bafb07a6b813abb466c711027262016109911e1650c91e4c0ce2bffec57b', 'page_no': [[15, 16, 17]]}", 'score': 0.13964016040104016}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'Doc_id': '460989726168196131', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '6 Klassifikationskriterien &gt; 6.2 Datenvernichtung nach DIN 66399 / ISO 21964-1', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[26, 27]]}", 'score': 0.30524582884691753}
+{'Doc_id': '460989726168196128', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung &gt; 5.3.4 Vertraulich (I3)', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[23, 24]]}", 'score': 0.033806447796842255}
+{'Doc_id': '460989726168196126', 'Metadata': "{'Date': '22-09-2025', 'Document_Name': 'KISTERS_IS_Klassifikation_ZutrittZugangZugriff.pdf', 'Section': '5 Zugriffskontrolle AND 5 Zugriffskontrolle &gt; 5.1 Klassifikation von Information AND 5 Zugriffskontrolle &gt; 5.2 Zugriffsberechtigungen AND 5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung AND 5 Zugriffskontrolle &gt; 5.3 Maßnahmen zur Zugriffskontrolle und Überwachung &gt; 5.3.1 Öffentlich (I0)', 'binary_hash': 'cbf90a11a32ddf5193d50cbaad55221c0d8caede783592f4ed3dfdb474a37f2c', 'page_no': [[19, 20, 21, 22]]}", 'score': 0.008008386791973297}
 </t>
   </si>
   <si>
@@ -276,7 +425,68 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">According to Source 2, the ISO 27019 standard provides a framework for information security. The provided documentation (ISO IEC 27002) outlines technical controls that can be implemented to achieve the objectives of the ISO 27019 standard. The documentation states that the cloud provider applies the procedures to address risks, but at least annually. The analysis, assessment and treatment of risks, including the approval of measures and acceptance of residual risks, are reviewed at least annually by the risk owners. [22]
+Therefore, the provided documentation indicates that the cloud provider uses controls based on the ISO 27019 standard, but it doesn't explicitly state that all controls from ISO 27019 are covered in the provided guidelines. [22]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerne! Organisation ist ein sehr breites Thema, aber ich kann dir eine Menge Informationen geben. Um dir besser helfen zu können, könntest du mir sagen, **was genau du wissen möchtest?** Hier sind ein paar Bereiche, in denen ich dir weiterhelfen kann:
+**1. Allgemeine Prinzipien der Organisation:**
+*   **Warum ist Organisation wichtig?** (Effizienz, Produktivität, Stressreduktion, Zieleerreichung)
+*   **Verschiedene Arten von Organisationen:** (persönliche, berufliche, gemeinschaftliche)
+*   **Grundlegende Prinzipien:** (Ziele definieren, Prioritäten setzen, Aufgaben delegieren, Zeitmanagement, Raum schaffen)
+*   **Die Bedeutung von Struktur und Flexibilität:** (eine gute Struktur hilft, aber Flexibilität ist wichtig, um sich an Veränderungen anzupassen)
+**2. Praktische Tipps und Techniken:**
+*   **Zeitmanagement:** (Pomodoro-Technik, Eisenhower-Matrix, To-Do-Listen, Zeitleisteneinteilung)
+*   **Aufgabenmanagement:** (Priorisierung, Aufgabenplanung, Aufgabenverteilung)
+*   **Raumgestaltung:** (Arbeitsplatzorganisation, Aufbewahrungssysteme, Minimalismus)
+*   **Digitale Organisation:** (Dateisysteme, Cloud-Speicher, Apps für Aufgabenmanagement)
+*   **Projekte organisieren:** (Projektplanung, Aufgabenverteilung, Fortschrittskontrolle)
+**3. Spezifische Bereiche:**
+*   **Persönliche Organisation:** (Aufgabenliste, Terminkalender, Gewohnheitsbildung)
+*   **Berufliche Organisation:** (Meetings planen, Dokumente organisieren, Informationen finden)
+*   **Kreative Organisation:** (Inspiration finden, Ideen sammeln, Projekte strukturieren)
+*   **Reiseorganisation:** (Reiseplanung, Gepäckpacken, Reiseunterlagen)
+**Um dir die bestmögliche Antwort zu geben, könntest du mir folgende Fragen beantworten:**
+*   **Was ist dein Ziel?** (Was möchtest du mit besserer Organisation erreichen?)
+*   **Welche Bereiche sind für dich am wichtigsten?** (Persönlich, beruflich, etc.)
+*   **Hast du bestimmte Probleme oder Herausforderungen?** (Was fällt dir besonders schwer?)
+*   **Hast du bestimmte Methoden bereits ausprobiert?** (Was hat funktioniert, was nicht?)
+Je mehr Informationen du mir gibst, desto besser kann ich dir helfen! Ich kann dir zum Beispiel:
+*   **Konkrete Tipps und Strategien geben.**
+*   **Tools und Apps empfehlen.**
+*   **Beispiele für gute Organisationsmethoden zeigen.**
+*   **Dir helfen, deine eigenen Organisationsstrategien zu entwickeln.**
+Lass mich wissen, womit ich dir helfen kann!
+**Sources:**
+*   Enwicklung und Änderung von Informationssystemen (DEV) 5.11 auf Seite 95
+*   Sicherstellen der Informationssicherheit im Entwicklungskreislauf von Systemkomponenten des Cloud-Dienstes
+*   Steuerung und Überwachung von Dienstleistern und Lieferanten (SSO) 5.12 auf Seite 101
+*   Sicherstellen des Schutzes von Informationen auf die Dienstleister bzw. Lieferanten des Cloud-Anbieters (Subdienstleister) zugreifen können, sowie Überwachung der vereinbarten Leistungen und Sicherheitsanforderungen
+*   Umgang mit Sicherheitsvorfällen (SIM) 5.13 auf Seite 106
+*   Gewährleisten eines konsistenten und umfassenden Vorgehens zur Erfassung, Bewertung, Kommunikation und Behandlung von Sicherheitsvorfällen
+*   Kontinuität des Geschäftsbetriebs und Notfallmanagement (bCM) 5.14 auf Seite 110
+*   Planen, Implementieren, Aufrechterhalten und Testen von Verfahren und Maßnahmen zur Kontinuität des Geschäftsbetriebs und für das Notfallmanagement
+*   Compliance (COM) 5.15 auf Seite 113
+*   Vermeiden von Verstößen gegen gesetzliche, regulatorische, selbstauferlegte oder vertragliche Anforderungen zur Informationssicherheit und Überprüfung der Einhaltung
+*   Umgang mit Ermittlungsanfragen staatlicher Stellen (INQ) 5.16 auf Seite 116
+*   Gewährleisten eines angemessenen Umgangs mit Ermittlungsanfragen staatlicher Stellen hinsichtlich juristischer Prüfung, Information der Cloud-Kunden und Begrenzung des Zugriffs auf oder der Offenlegung von Daten
+*   Produkt-Sicherheit (PSS) 5.17 auf Seite 118
+*   Bereitstellen aktueller Informationen zur sicheren Konfiguration und über bekannte Schwachstellen des Cloud-Dienstes für Cloud-Kunden, geeignete Mechanismen zur Fehlerbehandlung und Protokollierung sowie zur Authentisierung und Autorisierung von Benutzern der Cloud-Kunden
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die folgenden kryptografischen Standards sollten befolgt werden [6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 25, 26]. Diese Standards umfassen Empfehlungen und Schlüssellängen für verschiedene kryptografische Verfahren wie TLS, IPSec, SSH, sowie allgemeine Richtlinien für Key Management und die Verwendung von kryptografischen Modulen.  Zusätzlich werden spezifische Richtlinien für die Smart Metering PKI und Code Signing Zertifikate empfohlen [17, 22, 23, 24]. Die KISTERS Passwortrichtlinie und das Richtlinien zur technischen Schwächstellen-Governance sind ebenfalls relevant [15, 16].  Die BSI TR-03116 enthält kryptografische Vorgaben für Projekte der Bundesregierung [25].  Zufallszahlengeneratoren sollten ebenfalls verwendet werden [26].
+</t>
+  </si>
+  <si>
+    <t>Papierdokumente MÜSSEn mit Aktenvernichter der Klasse 4 geschreddert werden [3].</t>
+  </si>
+  <si>
     <t>0, 1, 2</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>N/A</t>
@@ -637,7 +847,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -680,22 +890,22 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -703,22 +913,22 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -729,22 +939,22 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -752,22 +962,22 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -778,31 +988,126 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" t="s">
-        <v>42</v>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>